<commit_message>
sample spreadsheet added, imageadded for items, displayed in all places where items are displayed
</commit_message>
<xml_diff>
--- a/client/public/ItemTemplate.xlsx
+++ b/client/public/ItemTemplate.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonyneher/Desktop/Home-Order-Spark/client/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lemon\Documents\Home-Order-Spark\client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD876C5-05E5-2449-A705-559C43EEBBFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2280" windowWidth="24740" windowHeight="11880" xr2:uid="{D7091829-A916-2549-9D9C-D56E99FFF2CA}"/>
+    <workbookView xWindow="0" yWindow="2280" windowWidth="24735" windowHeight="11880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="23">
   <si>
     <t>Item Name</t>
   </si>
@@ -86,34 +85,28 @@
     <t>Tools</t>
   </si>
   <si>
-    <t>pew pew</t>
-  </si>
-  <si>
-    <t>no rain here</t>
-  </si>
-  <si>
-    <t>Nice looking socket you got there</t>
-  </si>
-  <si>
-    <t>You want sum blue?</t>
-  </si>
-  <si>
-    <t>Gun 2</t>
-  </si>
-  <si>
-    <t>Umbrella 2</t>
-  </si>
-  <si>
-    <t>Socket 2</t>
-  </si>
-  <si>
-    <t>Blue 2</t>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>https://images-na.ssl-images-amazon.com/images/I/71mglRoZBKL._AC_SX679_.jpg</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>name 2</t>
+  </si>
+  <si>
+    <t>desc 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -467,19 +460,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D48060F-817E-6E4E-B3E8-72BFAD1E1921}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F3" sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,94 +489,73 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>300</v>
-      </c>
-      <c r="D2">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
         <v>18</v>
-      </c>
-      <c r="C3">
-        <v>3000000</v>
-      </c>
-      <c r="D3">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>40</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>5</v>
       </c>
@@ -591,7 +564,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>5</v>
       </c>
@@ -603,7 +576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>5</v>
       </c>
@@ -615,7 +588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>5</v>
       </c>
@@ -627,7 +600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>5</v>
       </c>
@@ -639,7 +612,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>5</v>
       </c>
@@ -651,7 +624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>5</v>
       </c>
@@ -659,7 +632,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>5</v>
       </c>
@@ -667,7 +640,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>5</v>
       </c>
@@ -675,7 +648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>5</v>
       </c>
@@ -683,7 +656,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>5</v>
       </c>
@@ -691,7 +664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>5</v>
       </c>
@@ -699,1434 +672,1434 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="19" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="20" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="21" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="22" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="23" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="24" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="25" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="26" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="27" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="28" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="29" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="30" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="31" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="5:65" x14ac:dyDescent="0.2">
+    <row r="32" spans="5:65" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E84" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E85" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E86" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E87" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E88" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E89" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E90" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E91" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E92" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E93" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E94" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E95" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E96" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E97" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E98" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E99" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E100" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E101" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E102" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E106" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E107" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E108" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E109" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E110" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E111" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E112" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E113" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E114" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E115" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E116" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E117" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E118" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E119" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E120" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E121" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E122" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E123" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E124" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E125" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E126" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E127" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E128" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E129" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E130" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E131" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E132" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E133" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E134" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E135" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E136" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E137" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E138" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E139" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E140" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E141" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="142" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E142" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E143" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="144" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E144" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="145" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E145" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="146" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E146" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="147" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E147" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="148" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E148" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="149" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E149" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="150" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E150" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="151" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E151" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="152" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E152" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="153" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E153" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="154" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E154" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="155" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E155" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="156" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E156" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="157" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E157" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="158" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E158" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="159" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E159" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="160" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E160" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E161" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E162" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="163" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E163" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="164" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E164" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="165" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E165" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E166" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E167" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E168" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E169" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="170" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E170" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="171" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E171" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E172" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="173" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E173" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="174" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E174" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="175" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E175" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="176" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E176" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="177" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E177" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="178" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E178" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="179" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E179" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="180" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E180" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="181" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E181" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="182" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E182" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="183" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E183" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="184" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E184" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="185" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E185" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="186" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E186" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="187" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E187" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="188" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E188" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="189" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E189" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="190" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E190" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="191" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E191" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="192" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E192" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E193" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E194" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E195" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E196" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E197" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E198" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E199" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E200" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E201" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E202" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E203" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E204" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E205" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E206" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E207" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E208" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E209" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E210" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E211" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E212" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E213" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E214" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E215" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E216" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E217" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E218" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E219" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E220" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="221" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="221" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E221" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="222" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="222" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E222" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="223" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="223" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E223" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="224" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="224" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E224" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="225" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E225" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="226" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E226" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="227" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E227" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="228" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E228" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="229" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E229" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="230" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E230" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="231" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E231" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="232" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E232" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="233" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E233" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="234" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E234" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="235" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E235" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="236" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E236" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="237" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E237" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="238" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E238" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="239" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E239" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="240" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E240" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="241" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E241" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="242" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E242" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="243" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E243" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="244" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E244" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="245" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E245" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="246" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E246" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="247" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E247" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="248" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E248" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="249" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E249" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="250" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E250" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="251" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E251" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="252" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="252" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E252" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="253" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E253" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="254" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="254" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E254" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="255" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E255" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="256" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="256" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E256" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="257" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E257" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="258" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E258" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="259" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E259" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="260" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="260" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E260" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="261" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="261" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E261" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="262" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="262" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E262" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="263" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="263" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E263" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="264" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="264" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E264" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="265" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="265" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E265" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="266" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="266" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E266" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="267" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="267" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E267" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="268" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="268" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E268" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="269" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="269" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E269" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="270" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E270" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="271" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="271" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E271" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="272" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="272" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E272" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="273" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="273" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E273" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="274" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="274" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E274" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="275" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="275" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E275" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="276" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="276" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E276" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="277" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="277" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E277" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="278" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="278" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E278" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="279" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="279" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E279" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="280" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="280" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E280" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="281" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="281" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E281" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="282" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E282" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="283" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="283" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E283" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="284" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="284" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E284" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="285" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="285" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E285" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="286" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="286" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E286" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="287" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="287" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E287" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="288" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="288" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E288" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="289" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="289" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E289" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="290" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="290" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E290" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="291" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="291" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E291" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="292" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="292" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E292" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="293" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="293" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E293" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="294" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="294" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E294" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="295" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="295" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E295" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="296" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="296" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E296" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="297" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="297" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E297" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="298" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="298" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E298" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="299" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="299" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E299" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="300" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E300" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="301" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E301" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="302" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E302" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="303" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="303" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E303" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E303" xr:uid="{0AA0408F-7411-E84C-878E-C49C440D2DB9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E303">
       <formula1>$BM$8:$BM$18</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed FAQ page, added route, aded to sign up page
</commit_message>
<xml_diff>
--- a/client/public/ItemTemplate.xlsx
+++ b/client/public/ItemTemplate.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="18">
   <si>
     <t>Item Name</t>
   </si>
@@ -86,21 +86,6 @@
   </si>
   <si>
     <t>Image</t>
-  </si>
-  <si>
-    <t>https://images-na.ssl-images-amazon.com/images/I/71mglRoZBKL._AC_SX679_.jpg</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>desc</t>
-  </si>
-  <si>
-    <t>name 2</t>
-  </si>
-  <si>
-    <t>desc 2</t>
   </si>
 </sst>
 </file>
@@ -464,7 +449,7 @@
   <dimension ref="A1:BM303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="A1:F3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -493,45 +478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="3" spans="1:65" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="J3" s="2"/>

</xml_diff>